<commit_message>
Tentativa de implementação de post de arquivo
</commit_message>
<xml_diff>
--- a/Projeto_ETS_OMIE_Back/StructureAndPrizes.xlsx
+++ b/Projeto_ETS_OMIE_Back/StructureAndPrizes.xlsx
@@ -38,16 +38,10 @@
     <t xml:space="preserve">110007405</t>
   </si>
   <si>
-    <t xml:space="preserve">111937242</t>
-  </si>
-  <si>
-    <t xml:space="preserve">111904125</t>
-  </si>
-  <si>
     <t xml:space="preserve">7114168</t>
   </si>
   <si>
-    <t xml:space="preserve">Total: 2106</t>
+    <t xml:space="preserve">Total: 5630.7</t>
   </si>
 </sst>
 </file>
@@ -388,10 +382,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>753</v>
+        <v>4199.7</v>
       </c>
     </row>
     <row r="3">
@@ -399,37 +393,15 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C3">
-        <v>300</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
+      <c r="C4" t="s">
         <v>5</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="C6" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mudanças com im plementação de manipulação do xml
</commit_message>
<xml_diff>
--- a/Projeto_ETS_OMIE_Back/StructureAndPrizes.xlsx
+++ b/Projeto_ETS_OMIE_Back/StructureAndPrizes.xlsx
@@ -32,16 +32,16 @@
     <t xml:space="preserve">Quantidade</t>
   </si>
   <si>
-    <t xml:space="preserve">Preços</t>
-  </si>
-  <si>
-    <t xml:space="preserve">110007405</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7114168</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total: 5630.7</t>
+    <t xml:space="preserve">Preços com Fator 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">111954114</t>
+  </si>
+  <si>
+    <t xml:space="preserve">111937242</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total: 5063.7</t>
   </si>
 </sst>
 </file>
@@ -385,7 +385,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>4199.7</v>
+        <v>269.7</v>
       </c>
     </row>
     <row r="3">
@@ -393,10 +393,10 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>1431</v>
+        <v>4794</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Projeto funcional com bug de download
</commit_message>
<xml_diff>
--- a/Projeto_ETS_OMIE_Back/StructureAndPrizes.xlsx
+++ b/Projeto_ETS_OMIE_Back/StructureAndPrizes.xlsx
@@ -41,7 +41,10 @@
     <t xml:space="preserve">111937242</t>
   </si>
   <si>
-    <t xml:space="preserve">Total: 5063.7</t>
+    <t xml:space="preserve">111954120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total: 5573.67</t>
   </si>
 </sst>
 </file>
@@ -400,8 +403,19 @@
       </c>
     </row>
     <row r="4">
-      <c r="C4" t="s">
+      <c r="A4" t="s">
         <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0.1</v>
+      </c>
+      <c r="C4">
+        <v>509.97</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>